<commit_message>
Updated BOM Rev A
</commit_message>
<xml_diff>
--- a/EL_Doorsign_PCB/EL_Doorsign_Bom_RevA.xlsx
+++ b/EL_Doorsign_PCB/EL_Doorsign_Bom_RevA.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\development\UWaterloo\EL_Doorsign\EL_Doorsign_PCB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDBEDA7C-504A-4164-94DB-80716964691D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17235" windowHeight="6480"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17235" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>QTY</t>
   </si>
@@ -126,12 +132,6 @@
     <t>TANT</t>
   </si>
   <si>
-    <t>AVX</t>
-  </si>
-  <si>
-    <t>TAJD-SERIES</t>
-  </si>
-  <si>
     <t>CAP_TANT_SIZE_D.G</t>
   </si>
   <si>
@@ -174,9 +174,6 @@
     <t>MMBT3904</t>
   </si>
   <si>
-    <t>MMPT3904FSCT-ND</t>
-  </si>
-  <si>
     <t>R1,R2,</t>
   </si>
   <si>
@@ -238,12 +235,30 @@
   </si>
   <si>
     <t>AP2210N-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>1276-1258-1-ND</t>
+  </si>
+  <si>
+    <t>Vishay Sprague</t>
+  </si>
+  <si>
+    <t>293D476X0016D2TE3</t>
+  </si>
+  <si>
+    <t>718-1086-1-ND</t>
+  </si>
+  <si>
+    <t>MMBT3904FSCT-ND</t>
+  </si>
+  <si>
+    <t>YAG2323CT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,12 +276,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -281,10 +302,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,6 +316,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -342,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,9 +400,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,6 +452,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,362 +644,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>0.99</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="Q4" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1.5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M5" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P5" t="s">
-        <v>31</v>
+      <c r="Q6" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J6">
-        <v>1.24</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2">
+        <v>603</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="2">
+        <v>6.94</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7">
-        <v>0.26</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="D11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8">
-        <v>603</v>
-      </c>
-      <c r="J8">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9">
-        <v>6.94</v>
-      </c>
-      <c r="O9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10">
-        <v>1.28</v>
-      </c>
-      <c r="O10" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="Q11" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11">
-        <v>0.62</v>
-      </c>
-      <c r="O11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -950,7 +1024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -962,7 +1036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>